<commit_message>
commited on april 15th
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/AgentInteractionReportData.xlsx
+++ b/ocms/src/test/resources/TestData/AgentInteractionReportData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD133E3-0095-4F01-8215-216C26F4B9DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22890" windowHeight="8040" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Show" sheetId="1" r:id="rId1"/>
@@ -14,9 +15,9 @@
     <sheet name="ExportReport" sheetId="3" r:id="rId5"/>
     <sheet name="ExportReportDateRange" sheetId="6" r:id="rId6"/>
     <sheet name="AdvanceSearch" sheetId="7" r:id="rId7"/>
+    <sheet name="Queries" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0" calcMode="manual"/>
-  <oleSize ref="A1:O24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="30">
   <si>
     <t>Report Channel</t>
   </si>
@@ -104,12 +105,85 @@
   </si>
   <si>
     <t>Media Agent3</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>15-04-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>SELECT M.[AgentID] as [Agent ID],A.[AgentName] as [Agent Name],A.[SupervisorName] as [Supervisor Name],[Channel],[Direction],[DNIS] as [Local Party],_x000D_
+[Ani] as [Remote Party],FORMAT([dbo].[VARCHARTODATETIME](M.ConnectedDateTime),'dd/MM/yyyy HH:mm:ss') as [Interaction Connected Date Time],_x000D_
+FORMAT([dbo].[VARCHARTODATETIME](M.[CreatedDateTime]),'dd/MM/yyyy HH:mm:ss') as [Created Date Time],[SessionID] as [Session ID],CONVERT(varchar, DATEADD(ms, M.QueueTime* 1000, 0), 108) as [Queue Time],_x000D_
+CONVERT(varchar, DATEADD(ms, M.ActiveTime* 1000, 0), 108) as [Active Time],_x000D_
+CONVERT(varchar, DATEADD(ms, M.HoldTime* 1000, 0), 108) as [Hold Time],_x000D_
+CONVERT(varchar, DATEADD(ms, M.ACWTime* 1000, 0), 108) as [ACW Time],_x000D_
+CONVERT(varchar, DATEADD(ms, M.HandleTime* 1000, 0), 108) as [Handle Time],_x000D_
+case when [IsConferenced]=1 Then 'true' when [IsConferenced]=0 then 'false' end as [Is Conferenced],_x000D_
+case when [IsTransfered]=1 Then 'true' when [IsTransfered]=0 then 'false' end as [Is Transfered], _x000D_
+[TPINTransferReconnected] as [TPIN Transfer Reconnected],[SubChannel] as [Sub Channel],_x000D_
+[SubSessionID] as [Sub Session ID],[InteractionID] as [Interaction ID],[Skill],[SkillName] as [Skill Name],_x000D_
+[DNISName] as [DNIS Name],[TransferedTo] as [Transfered To],[ConferencedTo] as [Conferenced To],_x000D_
+[ConferenceToAgentList] as [Conference To Agent List],[TransferToAgent] as [Transfer To Agent],_x000D_
+[TransferConferenceFromAgent] as [Transfer Conference From Agent] ,[TransferConferenceFromInteraction] as [Transfer Conference From Interaction],_x000D_
+--[OtherData],_x000D_
+FORMAT([dbo].[VARCHARTODATETIME](M.[ClosedDateTime]),'dd/MM/yyyy HH:mm:ss') as [Closed Date Time],_x000D_
+FORMAT([dbo].[VARCHARTODATETIME](M.[DisconnectedDateTime]),'dd/MM/yyyy HH:mm:ss') as [Interaction Disconnected Date Time],[ClosedReason] as [Closed Reason],_x000D_
+[CIF],[RegisteredMobileNo] as [Registered Mobile No] FROM (SELECT DISTINCT [User]  AS Ani,_x000D_
+							AgentId as AgentID,_x000D_
+							T.Channel,_x000D_
+							SubChannel,_x000D_
+							T.SessionID AS SessionID,_x000D_
+							SubSessionId as SubSessionID,_x000D_
+							InteractionId as InteractionID,_x000D_
+							T.Direction,_x000D_
+							CreatedDateTime,_x000D_
+							CreatedReason,_x000D_
+							Skill,_x000D_
+							TS.SkillName,_x000D_
+							ISNULL(A.FirstName,'') +' '+ ISNULL(A.LastName,'') AS AgentName,_x000D_
+							Dnis as DNIS,_x000D_
+							DnisName as DNISName,_x000D_
+							IsTransfered,_x000D_
+							IsConferenced,_x000D_
+							IsReconnected AS TPinTransferReconnected,_x000D_
+							IsConferencedTo AS ConferencedTo,_x000D_
+							IsTranferedTo AS TransferedTo,_x000D_
+							CASE WHEN IsTransfered=1 OR IsConferenced=1 THEN  TrasnferConferenceFromAgent ELSE '' END AS TransferConferenceFromAgent,_x000D_
+							CASE WHEN IsTransfered=1 OR IsConferenced=1 THEN  TrasnferConferenceFromInteraction ELSE '' END AS TransferConferenceFromInteraction,_x000D_
+							OtherData,_x000D_
+							ClosedDateTime AS ClosedDateTime,_x000D_
+							ClosedReason,_x000D_
+							CallConnectedTime AS  ConnectedDateTime,_x000D_
+							CallDisconnectedTime AS  DisconnectedDateTime,_x000D_
+							ActiveTime,_x000D_
+							HoldTime,_x000D_
+							TrasnferToAgent AS TransferToAgent,_x000D_
+							ConferenceToAgentList,_x000D_
+							QueueTime,_x000D_
+							AcwTime as ACWTime,_x000D_
+							ActiveTime+HoldTime+AcwTime HandleTime,_x000D_
+							IH.CIF,_x000D_
+							IH.CLID AS RegisteredMobileNo_x000D_
+							FROM TMAC_Interactions T with(nolock)_x000D_
+							INNER JOIN AGT_Agent A with(nolock) ON A.AvayaLoginID=T.AgentId _x000D_
+							LEFT JOIN AGT_Agent AA with(nolock) ON AA.AvayaLoginID = T.TrasnferConferenceFromAgent_x000D_
+							LEFT JOIN GBL_InteractionHistory IH WITH(NOLOCK) ON IH.SessionID=T.SessionId _x000D_
+							LEFT JOIN TMAC_Skills TS WITH(NOLOCK) ON TS.SkillExtension=T.Skill_x000D_
+							where 1=1 AND IH.ID IN (SELECT MIN(ID) FROM GBL_InteractionHistory WHERE SESSIONID=T.SessionId AND CLID IS NOT NULL)_x000D_
+							AND  ClosedDateTime&gt;='ReportBeforeDate' AND ClosedDateTime&lt;='ReportAfterDate') M_x000D_
+                            INNER JOIN  fn_AgentHierarchy('na','1','1') A  ON A.AgentId=M.AgentID_x000D_
+							order by M.[ClosedDateTime]</t>
+  </si>
+  <si>
+    <t>15-04-2020 15:30:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,9 +213,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,22 +499,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -471,25 +549,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +593,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -541,7 +619,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -567,7 +645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -593,7 +671,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -625,22 +703,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -674,23 +752,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,7 +785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -730,23 +808,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -763,7 +841,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -786,23 +864,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,7 +900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -848,26 +926,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="6" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="27.7265625" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="5" max="6" width="19.81640625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="9" max="9" width="24.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -896,7 +974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -923,6 +1001,69 @@
       </c>
       <c r="I2" t="s">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6D2C06-D0AE-4F83-B750-F2E25CDCB399}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commited on 16th April
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/AgentInteractionReportData.xlsx
+++ b/ocms/src/test/resources/TestData/AgentInteractionReportData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD133E3-0095-4F01-8215-216C26F4B9DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E1F9EE-F984-4A20-9299-0DFB23EECF29}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,71 +113,73 @@
     <t>15-04-2020 00:00:00</t>
   </si>
   <si>
-    <t>SELECT M.[AgentID] as [Agent ID],A.[AgentName] as [Agent Name],A.[SupervisorName] as [Supervisor Name],[Channel],[Direction],[DNIS] as [Local Party],_x000D_
-[Ani] as [Remote Party],FORMAT([dbo].[VARCHARTODATETIME](M.ConnectedDateTime),'dd/MM/yyyy HH:mm:ss') as [Interaction Connected Date Time],_x000D_
-FORMAT([dbo].[VARCHARTODATETIME](M.[CreatedDateTime]),'dd/MM/yyyy HH:mm:ss') as [Created Date Time],[SessionID] as [Session ID],CONVERT(varchar, DATEADD(ms, M.QueueTime* 1000, 0), 108) as [Queue Time],_x000D_
-CONVERT(varchar, DATEADD(ms, M.ActiveTime* 1000, 0), 108) as [Active Time],_x000D_
-CONVERT(varchar, DATEADD(ms, M.HoldTime* 1000, 0), 108) as [Hold Time],_x000D_
-CONVERT(varchar, DATEADD(ms, M.ACWTime* 1000, 0), 108) as [ACW Time],_x000D_
-CONVERT(varchar, DATEADD(ms, M.HandleTime* 1000, 0), 108) as [Handle Time],_x000D_
-case when [IsConferenced]=1 Then 'true' when [IsConferenced]=0 then 'false' end as [Is Conferenced],_x000D_
-case when [IsTransfered]=1 Then 'true' when [IsTransfered]=0 then 'false' end as [Is Transfered], _x000D_
-[TPINTransferReconnected] as [TPIN Transfer Reconnected],[SubChannel] as [Sub Channel],_x000D_
-[SubSessionID] as [Sub Session ID],[InteractionID] as [Interaction ID],[Skill],[SkillName] as [Skill Name],_x000D_
-[DNISName] as [DNIS Name],[TransferedTo] as [Transfered To],[ConferencedTo] as [Conferenced To],_x000D_
-[ConferenceToAgentList] as [Conference To Agent List],[TransferToAgent] as [Transfer To Agent],_x000D_
-[TransferConferenceFromAgent] as [Transfer Conference From Agent] ,[TransferConferenceFromInteraction] as [Transfer Conference From Interaction],_x000D_
---[OtherData],_x000D_
-FORMAT([dbo].[VARCHARTODATETIME](M.[ClosedDateTime]),'dd/MM/yyyy HH:mm:ss') as [Closed Date Time],_x000D_
-FORMAT([dbo].[VARCHARTODATETIME](M.[DisconnectedDateTime]),'dd/MM/yyyy HH:mm:ss') as [Interaction Disconnected Date Time],[ClosedReason] as [Closed Reason],_x000D_
-[CIF],[RegisteredMobileNo] as [Registered Mobile No] FROM (SELECT DISTINCT [User]  AS Ani,_x000D_
-							AgentId as AgentID,_x000D_
-							T.Channel,_x000D_
-							SubChannel,_x000D_
-							T.SessionID AS SessionID,_x000D_
-							SubSessionId as SubSessionID,_x000D_
-							InteractionId as InteractionID,_x000D_
-							T.Direction,_x000D_
-							CreatedDateTime,_x000D_
-							CreatedReason,_x000D_
-							Skill,_x000D_
-							TS.SkillName,_x000D_
-							ISNULL(A.FirstName,'') +' '+ ISNULL(A.LastName,'') AS AgentName,_x000D_
-							Dnis as DNIS,_x000D_
-							DnisName as DNISName,_x000D_
-							IsTransfered,_x000D_
-							IsConferenced,_x000D_
-							IsReconnected AS TPinTransferReconnected,_x000D_
-							IsConferencedTo AS ConferencedTo,_x000D_
-							IsTranferedTo AS TransferedTo,_x000D_
-							CASE WHEN IsTransfered=1 OR IsConferenced=1 THEN  TrasnferConferenceFromAgent ELSE '' END AS TransferConferenceFromAgent,_x000D_
-							CASE WHEN IsTransfered=1 OR IsConferenced=1 THEN  TrasnferConferenceFromInteraction ELSE '' END AS TransferConferenceFromInteraction,_x000D_
-							OtherData,_x000D_
-							ClosedDateTime AS ClosedDateTime,_x000D_
-							ClosedReason,_x000D_
-							CallConnectedTime AS  ConnectedDateTime,_x000D_
-							CallDisconnectedTime AS  DisconnectedDateTime,_x000D_
-							ActiveTime,_x000D_
-							HoldTime,_x000D_
-							TrasnferToAgent AS TransferToAgent,_x000D_
-							ConferenceToAgentList,_x000D_
-							QueueTime,_x000D_
-							AcwTime as ACWTime,_x000D_
-							ActiveTime+HoldTime+AcwTime HandleTime,_x000D_
-							IH.CIF,_x000D_
-							IH.CLID AS RegisteredMobileNo_x000D_
-							FROM TMAC_Interactions T with(nolock)_x000D_
-							INNER JOIN AGT_Agent A with(nolock) ON A.AvayaLoginID=T.AgentId _x000D_
-							LEFT JOIN AGT_Agent AA with(nolock) ON AA.AvayaLoginID = T.TrasnferConferenceFromAgent_x000D_
-							LEFT JOIN GBL_InteractionHistory IH WITH(NOLOCK) ON IH.SessionID=T.SessionId _x000D_
-							LEFT JOIN TMAC_Skills TS WITH(NOLOCK) ON TS.SkillExtension=T.Skill_x000D_
-							where 1=1 AND IH.ID IN (SELECT MIN(ID) FROM GBL_InteractionHistory WHERE SESSIONID=T.SessionId AND CLID IS NOT NULL)_x000D_
-							AND  ClosedDateTime&gt;='ReportBeforeDate' AND ClosedDateTime&lt;='ReportAfterDate') M_x000D_
-                            INNER JOIN  fn_AgentHierarchy('na','1','1') A  ON A.AgentId=M.AgentID_x000D_
+    <t>14-04-2020 00:00:00</t>
+  </si>
+  <si>
+    <t>SELECT M.[AgentID] as [Agent ID],A.[AgentName] as [Agent Name],A.[SupervisorName] as [Supervisor Name],[Channel],[Direction],[DNIS] as [Local Party],
+[Ani] as [Remote Party],FORMAT([dbo].[VARCHARTODATETIME](M.ConnectedDateTime),'dd/MM/yyyy HH:mm:ss') as [Interaction Connected Date Time],
+FORMAT([dbo].[VARCHARTODATETIME](M.[CreatedDateTime]),'dd/MM/yyyy HH:mm:ss') as [Created Date Time],[SessionID] as [Session ID],CONVERT(varchar, DATEADD(ms, M.QueueTime* 1000, 0), 108) as [Queue Time],
+CONVERT(varchar, DATEADD(ms, M.ActiveTime* 1000, 0), 108) as [Active Time],
+CONVERT(varchar, DATEADD(ms, M.HoldTime* 1000, 0), 108) as [Hold Time],
+CONVERT(varchar, DATEADD(ms, M.ACWTime* 1000, 0), 108) as [ACW Time],
+CONVERT(varchar, DATEADD(ms, M.HandleTime* 1000, 0), 108) as [Handle Time],
+case when [IsConferenced]=1 Then 'true' when [IsConferenced]=0 then 'false' end as [Is Conferenced],
+case when [IsTransfered]=1 Then 'true' when [IsTransfered]=0 then 'false' end as [Is Transfered], 
+[TPINTransferReconnected] as [TPIN Transfer Reconnected],[SubChannel] as [Sub Channel],
+[SubSessionID] as [Sub Session ID],[InteractionID] as [Interaction ID],[Skill],[SkillName] as [Skill Name],
+[DNISName] as [DNIS Name],[TransferedTo] as [Transfered To],[ConferencedTo] as [Conferenced To],
+[ConferenceToAgentList] as [Conference To Agent List],[TransferToAgent] as [Transfer To Agent],
+[TransferConferenceFromAgent] as [Transfer Conference From Agent] ,[TransferConferenceFromInteraction] as [Transfer Conference From Interaction],
+--[OtherData],
+FORMAT([dbo].[VARCHARTODATETIME](M.[ClosedDateTime]),'dd/MM/yyyy HH:mm:ss') as [Closed Date Time],
+FORMAT([dbo].[VARCHARTODATETIME](M.[DisconnectedDateTime]),'dd/MM/yyyy HH:mm:ss') as [Interaction Disconnected Date Time],[ClosedReason] as [Closed Reason]
+--[CIF],[RegisteredMobileNo] as [Registered Mobile No] 
+FROM 
+(SELECT DISTINCT [User]  AS Ani,
+							AgentId as AgentID,
+							T.Channel,
+							SubChannel,
+							T.SessionID AS SessionID,
+							SubSessionId as SubSessionID,
+							InteractionId as InteractionID,
+							T.Direction,
+							CreatedDateTime,
+							CreatedReason,
+							Skill,
+							TS.SkillName,
+							ISNULL(A.FirstName,'') +' '+ ISNULL(A.LastName,'') AS AgentName,
+							Dnis as DNIS,
+							DnisName as DNISName,
+							IsTransfered,
+							IsConferenced,
+							IsReconnected AS TPinTransferReconnected,
+							IsConferencedTo AS ConferencedTo,
+							IsTranferedTo AS TransferedTo,
+							CASE WHEN IsTransfered=1 OR IsConferenced=1 THEN  TrasnferConferenceFromAgent ELSE '' END AS TransferConferenceFromAgent,
+							CASE WHEN IsTransfered=1 OR IsConferenced=1 THEN  TrasnferConferenceFromInteraction ELSE '' END AS TransferConferenceFromInteraction,
+							OtherData,
+							ClosedDateTime AS ClosedDateTime,
+							ClosedReason,
+							CallConnectedTime AS  ConnectedDateTime,
+							CallDisconnectedTime AS  DisconnectedDateTime,
+							ActiveTime,
+							HoldTime,
+							TrasnferToAgent AS TransferToAgent,
+							ConferenceToAgentList,
+							QueueTime,
+							AcwTime as ACWTime,
+							ActiveTime+HoldTime+AcwTime HandleTime,
+							IH.CIF,
+							IH.CLID AS RegisteredMobileNo
+							FROM TMAC_Interactions T with(nolock)
+							INNER JOIN AGT_Agent A with(nolock) ON A.AvayaLoginID=T.AgentId 
+							LEFT JOIN AGT_Agent AA with(nolock) ON AA.AvayaLoginID = T.TrasnferConferenceFromAgent
+							LEFT JOIN GBL_InteractionHistory IH WITH(NOLOCK) ON IH.SessionID=T.SessionId 
+							LEFT JOIN TMAC_Skills TS WITH(NOLOCK) ON TS.SkillExtension=T.Skill
+							where 1=1 AND IH.ID IN (SELECT MIN(ID) FROM GBL_InteractionHistory WHERE SESSIONID=T.SessionId AND CLID IS NOT NULL)
+							AND  ClosedDateTime&gt;='20200414000000' AND ClosedDateTime&lt;='20200415000000') M
+                            INNER JOIN  fn_AgentHierarchy('na','1','1') A  ON A.AgentId=M.AgentID
 							order by M.[ClosedDateTime]</t>
-  </si>
-  <si>
-    <t>15-04-2020 15:30:00</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1015,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1057,13 +1059,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commits as of 18thMay
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/AgentInteractionReportData.xlsx
+++ b/ocms/src/test/resources/TestData/AgentInteractionReportData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="8040" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18030" windowHeight="8040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Show" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="AdvanceSearch" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="B1:I24"/>
+  <oleSize ref="A1:K24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -490,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -920,7 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>